<commit_message>
modified Datenkatalog of Milestone 2
</commit_message>
<xml_diff>
--- a/Docs/Abgabe MileStone 2/Datenkatalog.xlsx
+++ b/Docs/Abgabe MileStone 2/Datenkatalog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\InfoSys-Lab\Docs\Corvin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\hs-esslingen\Unterrichtsfächer\7. Semester\Infosys\GitRepo\InfoSys-Lab\Docs\Abgabe MileStone 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sebastian</author>
   </authors>
   <commentList>
-    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="C21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Welche Vorlesung findet zu welchen Blöcken statt, aktuell nicht planbar</t>
   </si>
   <si>
-    <t>SSWS</t>
-  </si>
-  <si>
     <t>kann … anbieten</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>String(50)</t>
   </si>
   <si>
-    <t>Anzahl der verlangten SWS im aktuellen Semester</t>
-  </si>
-  <si>
     <t>String(10)</t>
   </si>
   <si>
@@ -372,12 +366,87 @@
   </si>
   <si>
     <t xml:space="preserve">gehört zu </t>
+  </si>
+  <si>
+    <t>Zeitsemester</t>
+  </si>
+  <si>
+    <t>String(6)</t>
+  </si>
+  <si>
+    <t>Constraint (nicht alle Werte erlaubt)</t>
+  </si>
+  <si>
+    <t>Beschreibt die Zugehörigkeit des Eintrags zu einem zeitlichen Halbjahr (WS2017)</t>
+  </si>
+  <si>
+    <t>DWS</t>
+  </si>
+  <si>
+    <t>Anzahl der verlangten DWS im aktuellen Semester</t>
+  </si>
+  <si>
+    <t>Tätigkeiten</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Inkrementierte Nummer für jede Tätigkeit</t>
+  </si>
+  <si>
+    <t>Int(10)</t>
+  </si>
+  <si>
+    <t>Name der Tätigkeit</t>
+  </si>
+  <si>
+    <t>Anzahl der Studnen</t>
+  </si>
+  <si>
+    <t>Eine Tätigkeit ist ein Aufwand welcher von einem Dozenten übernommen wird</t>
+  </si>
+  <si>
+    <t>VorlesungPlan</t>
+  </si>
+  <si>
+    <t>VorlesungReal</t>
+  </si>
+  <si>
+    <t>Vorlesungsblock</t>
+  </si>
+  <si>
+    <t>Beschreibt eine Zeitspanne in welcher die Vorlesung gehalten wird</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Kombination aus Zeit und Tag</t>
+  </si>
+  <si>
+    <t>hat einen</t>
+  </si>
+  <si>
+    <t>ist einer…zugeordnet</t>
+  </si>
+  <si>
+    <t>hat</t>
+  </si>
+  <si>
+    <t>Tätigkeit</t>
+  </si>
+  <si>
+    <t>ist zugeordnet zu</t>
+  </si>
+  <si>
+    <t>ist eine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,7 +518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -465,6 +534,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -781,17 +856,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="2" max="2" width="80.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -810,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -854,15 +929,23 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,7 +960,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,11 +982,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,16 +1021,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="10">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -961,71 +1044,71 @@
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="9">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>17</v>
+      <c r="E5" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>31</v>
@@ -1035,9 +1118,11 @@
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="D7" s="9"/>
       <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1049,9 +1134,11 @@
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="D8" s="9"/>
       <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
@@ -1063,30 +1150,30 @@
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>17</v>
+      <c r="E9" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="8">
+        <v>101</v>
+      </c>
+      <c r="D10" s="10">
         <v>1</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -1094,7 +1181,106 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1102,19 +1288,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="4" width="44.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="73.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="9" max="9" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -1151,193 +1338,193 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
         <v>82</v>
       </c>
-      <c r="C9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" t="s">
-        <v>84</v>
-      </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1345,345 +1532,596 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
         <v>59</v>
       </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" t="s">
         <v>53</v>
       </c>
-      <c r="H13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>97</v>
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33" t="s">
+        <v>47</v>
+      </c>
+      <c r="I33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checked Tables for BCNF
</commit_message>
<xml_diff>
--- a/Docs/Abgabe MileStone 2/Datenkatalog.xlsx
+++ b/Docs/Abgabe MileStone 2/Datenkatalog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>ist eine</t>
+  </si>
+  <si>
+    <t>Zum Studiengang zugeordnete Fakultät</t>
+  </si>
+  <si>
+    <t>String (230)</t>
   </si>
 </sst>
 </file>
@@ -880,7 +886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -900,7 +906,7 @@
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -908,7 +914,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -940,7 +946,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>108</v>
       </c>
@@ -985,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,65 +1954,63 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" t="s">
         <v>45</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>67</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>59</v>
       </c>
-      <c r="E27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" t="s">
-        <v>47</v>
-      </c>
-      <c r="G27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" s="7" t="s">
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>46</v>
@@ -2022,63 +2026,65 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" t="s">
+      <c r="A30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" t="s">
         <v>0</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>112</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>49</v>
       </c>
-      <c r="E30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" t="s">
-        <v>47</v>
-      </c>
-      <c r="G30" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>106</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>113</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>55</v>
       </c>
-      <c r="E31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" t="s">
-        <v>47</v>
-      </c>
-      <c r="H31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" t="s">
-        <v>53</v>
-      </c>
       <c r="E32" t="s">
         <v>46</v>
       </c>
@@ -2086,7 +2092,7 @@
         <v>47</v>
       </c>
       <c r="G32" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H32" t="s">
         <v>47</v>
@@ -2095,32 +2101,56 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" t="s">
         <v>102</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>105</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>103</v>
       </c>
-      <c r="E33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" t="s">
-        <v>47</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H34" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>